<commit_message>
Added base for lid motor driver.
</commit_message>
<xml_diff>
--- a/docs/crossbar.xlsx
+++ b/docs/crossbar.xlsx
@@ -7,16 +7,15 @@
     <workbookView xWindow="0" yWindow="90" windowWidth="28755" windowHeight="12585"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="crossBar" sheetId="1" r:id="rId1"/>
+    <sheet name="Peripherals" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="55">
   <si>
     <t>PB10</t>
   </si>
@@ -91,6 +90,96 @@
   </si>
   <si>
     <t>Cap Sense</t>
+  </si>
+  <si>
+    <t>PA7</t>
+  </si>
+  <si>
+    <t>AF2</t>
+  </si>
+  <si>
+    <t>TIM3_CH2</t>
+  </si>
+  <si>
+    <t>TIM1_CH1</t>
+  </si>
+  <si>
+    <t>PB13</t>
+  </si>
+  <si>
+    <t>AF1</t>
+  </si>
+  <si>
+    <t>PE8</t>
+  </si>
+  <si>
+    <t>PE11</t>
+  </si>
+  <si>
+    <t>TIM1_CH2</t>
+  </si>
+  <si>
+    <t>PA9</t>
+  </si>
+  <si>
+    <t>PA10</t>
+  </si>
+  <si>
+    <t>TIM1_CH3</t>
+  </si>
+  <si>
+    <t>PE13</t>
+  </si>
+  <si>
+    <t>PA11</t>
+  </si>
+  <si>
+    <t>TIM1_CH4</t>
+  </si>
+  <si>
+    <t>PE14</t>
+  </si>
+  <si>
+    <t>LIS3DSH</t>
+  </si>
+  <si>
+    <t>USB</t>
+  </si>
+  <si>
+    <t>Lid Motor</t>
+  </si>
+  <si>
+    <t>Peripheral</t>
+  </si>
+  <si>
+    <t>TIM1</t>
+  </si>
+  <si>
+    <t>TIM2</t>
+  </si>
+  <si>
+    <t>Scheduler</t>
+  </si>
+  <si>
+    <t>I2C1</t>
+  </si>
+  <si>
+    <t>USART1</t>
+  </si>
+  <si>
+    <t>LEDs</t>
+  </si>
+  <si>
+    <t>AF7</t>
+  </si>
+  <si>
+    <t>USART1_TX</t>
+  </si>
+  <si>
+    <t>TIM1_CH1N</t>
+  </si>
+  <si>
+    <t>PE9</t>
   </si>
 </sst>
 </file>
@@ -431,19 +520,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1">
+    <row r="1" spans="1:12" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -456,150 +549,350 @@
       <c r="E1" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="G1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:12">
       <c r="A2">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3">
+        <v>42</v>
+      </c>
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4">
+        <v>44</v>
+      </c>
+      <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" t="s">
+        <v>36</v>
+      </c>
+      <c r="K4">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5">
+        <v>45</v>
+      </c>
+      <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" t="s">
+        <v>39</v>
+      </c>
+      <c r="K5">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6">
+        <v>96</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K6">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7">
+        <v>48</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" t="s">
+        <v>16</v>
+      </c>
+      <c r="K7">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8">
+        <v>52</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" t="s">
+        <v>53</v>
+      </c>
+      <c r="K8">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9">
+        <v>39</v>
+      </c>
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" t="s">
+        <v>53</v>
+      </c>
+      <c r="K9">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10">
+        <v>69</v>
+      </c>
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" t="s">
+        <v>36</v>
+      </c>
+      <c r="J10" t="s">
+        <v>42</v>
+      </c>
+      <c r="K10">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11">
+        <v>68</v>
+      </c>
+      <c r="B11" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" t="s">
+        <v>33</v>
+      </c>
+      <c r="J11" t="s">
+        <v>42</v>
+      </c>
+      <c r="K11">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12">
+        <v>95</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
+      <c r="H12" t="s">
+        <v>7</v>
+      </c>
+      <c r="L12">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13">
+        <v>93</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" t="s">
+        <v>15</v>
+      </c>
+      <c r="L13">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14">
         <v>67</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B14" t="s">
         <v>2</v>
       </c>
-      <c r="G2" t="s">
+      <c r="F14" t="s">
+        <v>28</v>
+      </c>
+      <c r="H14" t="s">
         <v>3</v>
       </c>
-      <c r="K2">
+      <c r="L14">
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
-      <c r="A3">
+    <row r="15" spans="1:12">
+      <c r="A15">
         <v>92</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B15" t="s">
         <v>4</v>
       </c>
-      <c r="G3" t="s">
+      <c r="D15" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" t="s">
+        <v>52</v>
+      </c>
+      <c r="H15" t="s">
         <v>7</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I15" t="s">
+        <v>52</v>
+      </c>
+      <c r="J15" t="s">
         <v>21</v>
       </c>
-      <c r="K3">
+      <c r="L15">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
-      <c r="A4">
-        <v>95</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" t="s">
-        <v>7</v>
-      </c>
-      <c r="K4">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5">
+    <row r="16" spans="1:12">
+      <c r="A16">
         <v>47</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B16" t="s">
         <v>0</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H16" t="s">
         <v>1</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J16" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
-      <c r="A6">
+    <row r="17" spans="1:12">
+      <c r="A17">
         <v>66</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B17" t="s">
         <v>10</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H17" t="s">
         <v>14</v>
       </c>
-      <c r="K6">
+      <c r="L17">
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
-      <c r="A7">
-        <v>93</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K7">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="A8">
-        <v>96</v>
-      </c>
-      <c r="B8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" t="s">
-        <v>15</v>
-      </c>
-      <c r="I8" t="s">
-        <v>20</v>
-      </c>
-      <c r="J8">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="A9">
-        <v>48</v>
-      </c>
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9" t="s">
-        <v>16</v>
-      </c>
-      <c r="J9">
-        <v>35</v>
+    <row r="18" spans="1:12">
+      <c r="A18">
+        <v>70</v>
+      </c>
+      <c r="B18" t="s">
+        <v>38</v>
+      </c>
+      <c r="F18" t="s">
+        <v>39</v>
+      </c>
+      <c r="J18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19">
+        <v>40</v>
+      </c>
+      <c r="B19" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" t="s">
+        <v>28</v>
+      </c>
+      <c r="K19">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:L18">
+    <sortCondition ref="K2:K18"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
@@ -607,24 +900,60 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="1" customFormat="1">
+      <c r="A1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added basic information for all of the connections
</commit_message>
<xml_diff>
--- a/docs/crossbar.xlsx
+++ b/docs/crossbar.xlsx
@@ -9,13 +9,14 @@
   <sheets>
     <sheet name="crossBar" sheetId="1" r:id="rId1"/>
     <sheet name="Peripherals" sheetId="2" r:id="rId2"/>
+    <sheet name="DMA" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="97">
   <si>
     <t>PB10</t>
   </si>
@@ -164,9 +165,6 @@
     <t>I2C1</t>
   </si>
   <si>
-    <t>USART1</t>
-  </si>
-  <si>
     <t>LEDs</t>
   </si>
   <si>
@@ -180,6 +178,135 @@
   </si>
   <si>
     <t>PE9</t>
+  </si>
+  <si>
+    <t>Hall Sensor 1</t>
+  </si>
+  <si>
+    <t>Hall Sensor 2</t>
+  </si>
+  <si>
+    <t>GPIO</t>
+  </si>
+  <si>
+    <t>Push 1</t>
+  </si>
+  <si>
+    <t>Push 2</t>
+  </si>
+  <si>
+    <t>PA0</t>
+  </si>
+  <si>
+    <t>FAN</t>
+  </si>
+  <si>
+    <t>Push Button</t>
+  </si>
+  <si>
+    <t>Accelerometer</t>
+  </si>
+  <si>
+    <t>TIM2_CH1</t>
+  </si>
+  <si>
+    <t>PA1</t>
+  </si>
+  <si>
+    <t>TIM2_CH2</t>
+  </si>
+  <si>
+    <t>Fan</t>
+  </si>
+  <si>
+    <t>Pump</t>
+  </si>
+  <si>
+    <t>PA6</t>
+  </si>
+  <si>
+    <t>TIM3_CH1</t>
+  </si>
+  <si>
+    <t>PB4</t>
+  </si>
+  <si>
+    <t>TIM3</t>
+  </si>
+  <si>
+    <t>TIM4</t>
+  </si>
+  <si>
+    <t>CS_IRQ</t>
+  </si>
+  <si>
+    <t>PE15</t>
+  </si>
+  <si>
+    <t>PB12</t>
+  </si>
+  <si>
+    <t>PA2</t>
+  </si>
+  <si>
+    <t>USART2_TX</t>
+  </si>
+  <si>
+    <t>Peripheral Requests</t>
+  </si>
+  <si>
+    <t>Stream 0</t>
+  </si>
+  <si>
+    <t>Stream 7</t>
+  </si>
+  <si>
+    <t>Stream 6</t>
+  </si>
+  <si>
+    <t>Stream 5</t>
+  </si>
+  <si>
+    <t>Stream 4</t>
+  </si>
+  <si>
+    <t>Stream 3</t>
+  </si>
+  <si>
+    <t>Stream 2</t>
+  </si>
+  <si>
+    <t>Stream 1</t>
+  </si>
+  <si>
+    <t>Channel 0</t>
+  </si>
+  <si>
+    <t>Channel 1</t>
+  </si>
+  <si>
+    <t>Channel 2</t>
+  </si>
+  <si>
+    <t>Channel 3</t>
+  </si>
+  <si>
+    <t>Channel 4</t>
+  </si>
+  <si>
+    <t>Channel 5</t>
+  </si>
+  <si>
+    <t>Channel 6</t>
+  </si>
+  <si>
+    <t>Channel 7</t>
+  </si>
+  <si>
+    <t>DMA1</t>
+  </si>
+  <si>
+    <t>USART2</t>
   </si>
 </sst>
 </file>
@@ -203,12 +330,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -223,9 +356,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -520,29 +656,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1">
+    <row r="1" spans="1:12" s="3" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="C1" s="1"/>
       <c r="D1" s="1" t="s">
         <v>22</v>
       </c>
@@ -559,7 +695,7 @@
         <v>9</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>17</v>
@@ -572,326 +708,544 @@
       </c>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2">
-        <v>32</v>
-      </c>
-      <c r="B2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" t="s">
-        <v>27</v>
-      </c>
-      <c r="J2" t="s">
-        <v>41</v>
-      </c>
-      <c r="K2">
-        <v>17</v>
-      </c>
+      <c r="A2" s="2">
+        <v>23</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="K2" s="2">
+        <v>12</v>
+      </c>
+      <c r="L2" s="2"/>
     </row>
     <row r="3" spans="1:12">
       <c r="A3">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="D3" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="E3" t="s">
-        <v>33</v>
+        <v>65</v>
       </c>
       <c r="F3" t="s">
-        <v>33</v>
+        <v>65</v>
       </c>
       <c r="K3">
-        <v>29</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D4" t="s">
-        <v>43</v>
+        <v>76</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="E4" t="s">
+        <v>77</v>
+      </c>
+      <c r="I4" t="s">
+        <v>77</v>
+      </c>
+      <c r="K4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="2">
+        <v>69</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F4" t="s">
-        <v>36</v>
-      </c>
-      <c r="K4">
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K5" s="2">
+        <v>41</v>
+      </c>
+      <c r="L5" s="2"/>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="2">
+        <v>70</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="2">
         <v>31</v>
       </c>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="A5">
-        <v>45</v>
-      </c>
-      <c r="B5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F5" t="s">
-        <v>39</v>
-      </c>
-      <c r="K5">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6">
-        <v>96</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" t="s">
-        <v>15</v>
-      </c>
-      <c r="J6" t="s">
-        <v>20</v>
-      </c>
-      <c r="K6">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="A7">
-        <v>48</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7" t="s">
-        <v>16</v>
-      </c>
-      <c r="K7">
-        <v>35</v>
-      </c>
+      <c r="B7" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="K7" s="2">
+        <v>18</v>
+      </c>
+      <c r="L7" s="2"/>
     </row>
     <row r="8" spans="1:12">
       <c r="A8">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" t="s">
-        <v>53</v>
+        <v>25</v>
+      </c>
+      <c r="G8" t="s">
+        <v>27</v>
+      </c>
+      <c r="J8" t="s">
+        <v>41</v>
       </c>
       <c r="K8">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9">
-        <v>39</v>
+        <v>67</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" t="s">
+        <v>28</v>
+      </c>
+      <c r="H9" t="s">
+        <v>3</v>
+      </c>
+      <c r="L9">
         <v>43</v>
       </c>
-      <c r="E9" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" t="s">
-        <v>53</v>
-      </c>
-      <c r="K9">
-        <v>39</v>
-      </c>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10">
-        <v>69</v>
-      </c>
-      <c r="B10" t="s">
-        <v>35</v>
-      </c>
-      <c r="F10" t="s">
-        <v>36</v>
-      </c>
-      <c r="J10" t="s">
+      <c r="A10" s="2">
+        <v>68</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="J10" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="K10">
-        <v>41</v>
-      </c>
+      <c r="K10" s="2">
+        <v>44</v>
+      </c>
+      <c r="L10" s="2"/>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11">
-        <v>68</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="A11" s="2">
+        <v>96</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K11" s="2">
         <v>34</v>
       </c>
-      <c r="F11" t="s">
-        <v>33</v>
-      </c>
-      <c r="J11" t="s">
-        <v>42</v>
-      </c>
-      <c r="K11">
-        <v>44</v>
-      </c>
+      <c r="L11" s="2"/>
     </row>
     <row r="12" spans="1:12">
-      <c r="A12">
-        <v>95</v>
-      </c>
-      <c r="B12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" t="s">
-        <v>24</v>
-      </c>
-      <c r="E12" t="s">
-        <v>7</v>
-      </c>
-      <c r="H12" t="s">
-        <v>7</v>
-      </c>
-      <c r="L12">
-        <v>19</v>
-      </c>
+      <c r="A12" s="2">
+        <v>47</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
     </row>
     <row r="13" spans="1:12">
       <c r="A13">
-        <v>93</v>
+        <v>48</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D13" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="E13" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
       <c r="H13" t="s">
-        <v>15</v>
-      </c>
-      <c r="L13">
-        <v>24</v>
+        <v>16</v>
+      </c>
+      <c r="K13">
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:12">
       <c r="A14">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="B14" t="s">
-        <v>2</v>
-      </c>
-      <c r="F14" t="s">
-        <v>28</v>
-      </c>
-      <c r="H14" t="s">
-        <v>3</v>
-      </c>
-      <c r="L14">
-        <v>43</v>
+        <v>75</v>
+      </c>
+      <c r="D14" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" t="s">
+        <v>56</v>
+      </c>
+      <c r="K14">
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:12">
       <c r="A15">
-        <v>92</v>
+        <v>52</v>
       </c>
       <c r="B15" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="D15" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="E15" t="s">
+        <v>56</v>
+      </c>
+      <c r="F15" t="s">
         <v>52</v>
       </c>
-      <c r="H15" t="s">
-        <v>7</v>
-      </c>
-      <c r="I15" t="s">
-        <v>52</v>
-      </c>
-      <c r="J15" t="s">
-        <v>21</v>
-      </c>
-      <c r="L15">
-        <v>23</v>
+      <c r="K15">
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="A16">
-        <v>47</v>
+        <v>90</v>
       </c>
       <c r="B16" t="s">
-        <v>0</v>
-      </c>
-      <c r="H16" t="s">
-        <v>1</v>
-      </c>
-      <c r="J16" t="s">
-        <v>20</v>
+        <v>70</v>
+      </c>
+      <c r="D16" t="s">
+        <v>67</v>
+      </c>
+      <c r="E16" t="s">
+        <v>69</v>
+      </c>
+      <c r="G16" t="s">
+        <v>69</v>
+      </c>
+      <c r="L16">
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:12">
-      <c r="A17">
-        <v>66</v>
-      </c>
-      <c r="B17" t="s">
-        <v>10</v>
-      </c>
-      <c r="H17" t="s">
-        <v>14</v>
-      </c>
-      <c r="L17">
-        <v>46</v>
+      <c r="A17" s="2">
+        <v>92</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2">
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:12">
       <c r="A18">
-        <v>70</v>
+        <v>93</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
-      </c>
-      <c r="F18" t="s">
-        <v>39</v>
-      </c>
-      <c r="J18" t="s">
-        <v>42</v>
+        <v>11</v>
+      </c>
+      <c r="D18" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" t="s">
+        <v>15</v>
+      </c>
+      <c r="H18" t="s">
+        <v>15</v>
+      </c>
+      <c r="L18">
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:12">
       <c r="A19">
+        <v>95</v>
+      </c>
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" t="s">
+        <v>7</v>
+      </c>
+      <c r="H19" t="s">
+        <v>7</v>
+      </c>
+      <c r="L19">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20">
+        <v>66</v>
+      </c>
+      <c r="B20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" t="s">
+        <v>73</v>
+      </c>
+      <c r="E20" t="s">
+        <v>56</v>
+      </c>
+      <c r="H20" t="s">
+        <v>14</v>
+      </c>
+      <c r="L20">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21">
+        <v>42</v>
+      </c>
+      <c r="B21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" t="s">
+        <v>33</v>
+      </c>
+      <c r="F21" t="s">
+        <v>33</v>
+      </c>
+      <c r="K21">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22">
+        <v>44</v>
+      </c>
+      <c r="B22" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" t="s">
+        <v>36</v>
+      </c>
+      <c r="F22" t="s">
+        <v>36</v>
+      </c>
+      <c r="K22">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23">
+        <v>45</v>
+      </c>
+      <c r="B23" t="s">
         <v>40</v>
       </c>
-      <c r="B19" t="s">
-        <v>54</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="D23" t="s">
         <v>43</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E23" t="s">
+        <v>39</v>
+      </c>
+      <c r="F23" t="s">
+        <v>39</v>
+      </c>
+      <c r="K23">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24">
+        <v>46</v>
+      </c>
+      <c r="B24" t="s">
+        <v>74</v>
+      </c>
+      <c r="K24">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25">
+        <v>39</v>
+      </c>
+      <c r="B25" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25" t="s">
+        <v>58</v>
+      </c>
+      <c r="E25" t="s">
+        <v>56</v>
+      </c>
+      <c r="F25" t="s">
+        <v>52</v>
+      </c>
+      <c r="K25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26">
+        <v>40</v>
+      </c>
+      <c r="B26" t="s">
+        <v>53</v>
+      </c>
+      <c r="D26" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" t="s">
         <v>28</v>
       </c>
-      <c r="K19">
+      <c r="F26" t="s">
+        <v>28</v>
+      </c>
+      <c r="K26">
         <v>27</v>
       </c>
     </row>
+    <row r="27" spans="1:12">
+      <c r="A27" s="2">
+        <v>30</v>
+      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="K27" s="2">
+        <v>15</v>
+      </c>
+      <c r="L27" s="2"/>
+    </row>
   </sheetData>
-  <sortState ref="A2:L18">
-    <sortCondition ref="K2:K18"/>
+  <sortState ref="A2:L26">
+    <sortCondition ref="B2:B26"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -900,10 +1254,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -933,27 +1287,137 @@
         <v>46</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B7" t="s">
         <v>49</v>
-      </c>
-      <c r="B5" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L9"/>
+  <sheetViews>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="1" customFormat="1">
+      <c r="B1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" t="s">
+        <v>87</v>
+      </c>
+      <c r="L2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" t="s">
+        <v>91</v>
+      </c>
+      <c r="I6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
moved lid motor and push button pins
</commit_message>
<xml_diff>
--- a/docs/crossbar.xlsx
+++ b/docs/crossbar.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="101">
   <si>
     <t>PB10</t>
   </si>
@@ -307,6 +307,18 @@
   </si>
   <si>
     <t>USART2</t>
+  </si>
+  <si>
+    <t>Lid Motor -FH</t>
+  </si>
+  <si>
+    <t>Lid Motor -RL</t>
+  </si>
+  <si>
+    <t>Lid Motor -RH</t>
+  </si>
+  <si>
+    <t>Lid Motor -FL</t>
   </si>
 </sst>
 </file>
@@ -658,7 +670,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -1118,7 +1132,7 @@
         <v>32</v>
       </c>
       <c r="D21" t="s">
-        <v>43</v>
+        <v>98</v>
       </c>
       <c r="E21" t="s">
         <v>33</v>
@@ -1138,7 +1152,7 @@
         <v>37</v>
       </c>
       <c r="D22" t="s">
-        <v>43</v>
+        <v>99</v>
       </c>
       <c r="E22" t="s">
         <v>36</v>
@@ -1158,7 +1172,7 @@
         <v>40</v>
       </c>
       <c r="D23" t="s">
-        <v>43</v>
+        <v>100</v>
       </c>
       <c r="E23" t="s">
         <v>39</v>
@@ -1209,7 +1223,7 @@
         <v>53</v>
       </c>
       <c r="D26" t="s">
-        <v>43</v>
+        <v>97</v>
       </c>
       <c r="E26" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
added files for integration testing of timerDriver
</commit_message>
<xml_diff>
--- a/docs/crossbar.xlsx
+++ b/docs/crossbar.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\delibero.michael\personal\roboCooler\docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="90" windowWidth="28755" windowHeight="12585"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="106">
   <si>
     <t>PB10</t>
   </si>
@@ -159,9 +164,6 @@
     <t>TIM2</t>
   </si>
   <si>
-    <t>Scheduler</t>
-  </si>
-  <si>
     <t>I2C1</t>
   </si>
   <si>
@@ -180,27 +182,12 @@
     <t>PE9</t>
   </si>
   <si>
-    <t>Hall Sensor 1</t>
-  </si>
-  <si>
-    <t>Hall Sensor 2</t>
-  </si>
-  <si>
     <t>GPIO</t>
   </si>
   <si>
-    <t>Push 1</t>
-  </si>
-  <si>
-    <t>Push 2</t>
-  </si>
-  <si>
     <t>PA0</t>
   </si>
   <si>
-    <t>FAN</t>
-  </si>
-  <si>
     <t>Push Button</t>
   </si>
   <si>
@@ -237,9 +224,6 @@
     <t>TIM4</t>
   </si>
   <si>
-    <t>CS_IRQ</t>
-  </si>
-  <si>
     <t>PE15</t>
   </si>
   <si>
@@ -309,23 +293,59 @@
     <t>USART2</t>
   </si>
   <si>
-    <t>Lid Motor -FH</t>
-  </si>
-  <si>
-    <t>Lid Motor -RL</t>
-  </si>
-  <si>
-    <t>Lid Motor -RH</t>
-  </si>
-  <si>
-    <t>Lid Motor -FL</t>
+    <t>Timer</t>
+  </si>
+  <si>
+    <t>PD12</t>
+  </si>
+  <si>
+    <t>TIM4_CH1</t>
+  </si>
+  <si>
+    <t>TIM4_CH2</t>
+  </si>
+  <si>
+    <t>PD13</t>
+  </si>
+  <si>
+    <t>TIM4_CH3</t>
+  </si>
+  <si>
+    <t>PD14</t>
+  </si>
+  <si>
+    <t>TIM4_CH4</t>
+  </si>
+  <si>
+    <t>PD15</t>
+  </si>
+  <si>
+    <t>PB9</t>
+  </si>
+  <si>
+    <t>Green LED</t>
+  </si>
+  <si>
+    <t>SDA</t>
+  </si>
+  <si>
+    <t>Orange LED</t>
+  </si>
+  <si>
+    <t>Red LED</t>
+  </si>
+  <si>
+    <t>Blue LED</t>
+  </si>
+  <si>
+    <t>TIMER INT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -368,18 +388,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -426,7 +455,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -458,9 +487,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -492,6 +522,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -667,14 +698,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
@@ -685,7 +714,7 @@
     <col min="13" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1">
+    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -709,7 +738,7 @@
         <v>9</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>17</v>
@@ -721,82 +750,83 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="K2" s="2">
         <v>12</v>
       </c>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E3" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F3" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="K3">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
-      <c r="A4">
-        <v>25</v>
-      </c>
-      <c r="B4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E4" t="s">
-        <v>77</v>
-      </c>
-      <c r="I4" t="s">
-        <v>77</v>
-      </c>
-      <c r="K4">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>69</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K4" s="2">
+        <v>41</v>
+      </c>
+      <c r="L4" s="2"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
@@ -804,58 +834,52 @@
       <c r="J5" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="K5" s="2">
-        <v>41</v>
-      </c>
+      <c r="K5" s="2"/>
       <c r="L5" s="2"/>
     </row>
-    <row r="6" spans="1:12">
-      <c r="A6" s="2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" t="s">
         <v>70</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="I6" t="s">
+        <v>70</v>
+      </c>
+      <c r="K6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>31</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="K7" s="2">
         <v>18</v>
       </c>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>32</v>
       </c>
@@ -872,7 +896,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>67</v>
       </c>
@@ -889,7 +913,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>68</v>
       </c>
@@ -905,7 +929,7 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>42</v>
@@ -915,7 +939,7 @@
       </c>
       <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>96</v>
       </c>
@@ -939,7 +963,7 @@
       </c>
       <c r="L11" s="2"/>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>47</v>
       </c>
@@ -961,18 +985,15 @@
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>48</v>
       </c>
       <c r="B13" t="s">
         <v>13</v>
       </c>
-      <c r="D13" t="s">
-        <v>54</v>
-      </c>
       <c r="E13" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H13" t="s">
         <v>16</v>
@@ -981,64 +1002,55 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>51</v>
       </c>
       <c r="B14" t="s">
-        <v>75</v>
-      </c>
-      <c r="D14" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="E14" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="K14">
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>52</v>
       </c>
       <c r="B15" t="s">
         <v>29</v>
       </c>
-      <c r="D15" t="s">
-        <v>57</v>
-      </c>
       <c r="E15" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K15">
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>90</v>
       </c>
       <c r="B16" t="s">
-        <v>70</v>
-      </c>
-      <c r="D16" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E16" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="G16" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="L16">
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>92</v>
       </c>
@@ -1049,12 +1061,14 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
+      <c r="G17" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="H17" s="2" t="s">
         <v>7</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J17" s="2" t="s">
         <v>21</v>
@@ -1064,7 +1078,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>93</v>
       </c>
@@ -1072,11 +1086,14 @@
         <v>11</v>
       </c>
       <c r="D18" t="s">
-        <v>24</v>
+        <v>105</v>
       </c>
       <c r="E18" t="s">
         <v>15</v>
       </c>
+      <c r="G18" t="s">
+        <v>93</v>
+      </c>
       <c r="H18" t="s">
         <v>15</v>
       </c>
@@ -1084,19 +1101,19 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>95</v>
       </c>
       <c r="B19" t="s">
         <v>8</v>
       </c>
-      <c r="D19" t="s">
-        <v>24</v>
-      </c>
       <c r="E19" t="s">
         <v>7</v>
       </c>
+      <c r="G19" t="s">
+        <v>95</v>
+      </c>
       <c r="H19" t="s">
         <v>7</v>
       </c>
@@ -1104,162 +1121,265 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
-      <c r="A20">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>96</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21">
         <v>66</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>10</v>
       </c>
-      <c r="D20" t="s">
-        <v>73</v>
-      </c>
-      <c r="E20" t="s">
+      <c r="E21" t="s">
+        <v>53</v>
+      </c>
+      <c r="H21" t="s">
+        <v>14</v>
+      </c>
+      <c r="L21">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>59</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="K22" s="2">
+        <v>44</v>
+      </c>
+      <c r="L22" s="2"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>60</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="K23" s="2">
+        <v>45</v>
+      </c>
+      <c r="L23" s="2"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>61</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="K24" s="2">
+        <v>46</v>
+      </c>
+      <c r="L24" s="2"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>62</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="K25" s="2">
+        <v>47</v>
+      </c>
+      <c r="L25" s="2"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>42</v>
+      </c>
+      <c r="B26" t="s">
+        <v>32</v>
+      </c>
+      <c r="E26" t="s">
+        <v>33</v>
+      </c>
+      <c r="F26" t="s">
+        <v>33</v>
+      </c>
+      <c r="K26">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>44</v>
+      </c>
+      <c r="B27" t="s">
+        <v>37</v>
+      </c>
+      <c r="E27" t="s">
+        <v>36</v>
+      </c>
+      <c r="F27" t="s">
+        <v>36</v>
+      </c>
+      <c r="K27">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>45</v>
+      </c>
+      <c r="B28" t="s">
+        <v>40</v>
+      </c>
+      <c r="E28" t="s">
+        <v>39</v>
+      </c>
+      <c r="F28" t="s">
+        <v>39</v>
+      </c>
+      <c r="K28">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>46</v>
+      </c>
+      <c r="B29" t="s">
+        <v>67</v>
+      </c>
+      <c r="D29" s="5"/>
+      <c r="K29">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>39</v>
+      </c>
+      <c r="B30" t="s">
+        <v>31</v>
+      </c>
+      <c r="E30" t="s">
+        <v>53</v>
+      </c>
+      <c r="F30" t="s">
+        <v>51</v>
+      </c>
+      <c r="K30">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>40</v>
+      </c>
+      <c r="B31" t="s">
+        <v>52</v>
+      </c>
+      <c r="E31" t="s">
+        <v>28</v>
+      </c>
+      <c r="F31" t="s">
+        <v>28</v>
+      </c>
+      <c r="K31">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>30</v>
+      </c>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="H20" t="s">
-        <v>14</v>
-      </c>
-      <c r="L20">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12">
-      <c r="A21">
-        <v>42</v>
-      </c>
-      <c r="B21" t="s">
-        <v>32</v>
-      </c>
-      <c r="D21" t="s">
-        <v>98</v>
-      </c>
-      <c r="E21" t="s">
-        <v>33</v>
-      </c>
-      <c r="F21" t="s">
-        <v>33</v>
-      </c>
-      <c r="K21">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12">
-      <c r="A22">
-        <v>44</v>
-      </c>
-      <c r="B22" t="s">
-        <v>37</v>
-      </c>
-      <c r="D22" t="s">
-        <v>99</v>
-      </c>
-      <c r="E22" t="s">
-        <v>36</v>
-      </c>
-      <c r="F22" t="s">
-        <v>36</v>
-      </c>
-      <c r="K22">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12">
-      <c r="A23">
-        <v>45</v>
-      </c>
-      <c r="B23" t="s">
-        <v>40</v>
-      </c>
-      <c r="D23" t="s">
-        <v>100</v>
-      </c>
-      <c r="E23" t="s">
-        <v>39</v>
-      </c>
-      <c r="F23" t="s">
-        <v>39</v>
-      </c>
-      <c r="K23">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12">
-      <c r="A24">
-        <v>46</v>
-      </c>
-      <c r="B24" t="s">
-        <v>74</v>
-      </c>
-      <c r="K24">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12">
-      <c r="A25">
-        <v>39</v>
-      </c>
-      <c r="B25" t="s">
-        <v>31</v>
-      </c>
-      <c r="D25" t="s">
-        <v>58</v>
-      </c>
-      <c r="E25" t="s">
-        <v>56</v>
-      </c>
-      <c r="F25" t="s">
-        <v>52</v>
-      </c>
-      <c r="K25">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12">
-      <c r="A26">
-        <v>40</v>
-      </c>
-      <c r="B26" t="s">
-        <v>53</v>
-      </c>
-      <c r="D26" t="s">
-        <v>97</v>
-      </c>
-      <c r="E26" t="s">
-        <v>28</v>
-      </c>
-      <c r="F26" t="s">
-        <v>28</v>
-      </c>
-      <c r="K26">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12">
-      <c r="A27" s="2">
-        <v>30</v>
-      </c>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="K27" s="2">
+      <c r="K32" s="2">
         <v>15</v>
       </c>
-      <c r="L27" s="2"/>
+      <c r="L32" s="2"/>
     </row>
   </sheetData>
-  <sortState ref="A2:L26">
-    <sortCondition ref="B2:B26"/>
+  <sortState ref="A2:L35">
+    <sortCondition ref="B2:B35"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1267,20 +1387,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView topLeftCell="A2" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>44</v>
       </c>
@@ -1288,7 +1408,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>45</v>
       </c>
@@ -1296,44 +1416,44 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>46</v>
       </c>
       <c r="B3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>72</v>
-      </c>
       <c r="B5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>48</v>
       </c>
       <c r="B6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1343,92 +1463,90 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
-    </sheetView>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>80</v>
+      </c>
+      <c r="L2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>84</v>
+      </c>
+      <c r="I6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>86</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12">
-      <c r="A2" t="s">
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>87</v>
-      </c>
-      <c r="L2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
-      <c r="A3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="A4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="A5" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6" t="s">
-        <v>91</v>
-      </c>
-      <c r="I6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="A7" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="A8" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="A9" t="s">
-        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
reserved PE15 for timer integration test output
</commit_message>
<xml_diff>
--- a/docs/crossbar.xlsx
+++ b/docs/crossbar.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="107">
   <si>
     <t>PB10</t>
   </si>
@@ -339,6 +339,9 @@
   </si>
   <si>
     <t>TIMER INT</t>
+  </si>
+  <si>
+    <t>TIMER DRIVER INT</t>
   </si>
 </sst>
 </file>
@@ -388,13 +391,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -701,11 +703,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
@@ -1086,7 +1090,7 @@
         <v>11</v>
       </c>
       <c r="D18" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E18" t="s">
         <v>15</v>
@@ -1316,7 +1320,9 @@
       <c r="B29" t="s">
         <v>67</v>
       </c>
-      <c r="D29" s="5"/>
+      <c r="D29" t="s">
+        <v>105</v>
+      </c>
       <c r="K29">
         <v>33</v>
       </c>

</xml_diff>

<commit_message>
Added pushbuttons to layout
</commit_message>
<xml_diff>
--- a/docs/crossbar.xlsx
+++ b/docs/crossbar.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\delibero.michael\personal\roboCooler\docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="90" windowWidth="28755" windowHeight="12585"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="114">
   <si>
     <t>PB10</t>
   </si>
@@ -349,13 +354,22 @@
   </si>
   <si>
     <t>Timer Driver Int</t>
+  </si>
+  <si>
+    <t>PD11</t>
+  </si>
+  <si>
+    <t>PD9</t>
+  </si>
+  <si>
+    <t>USART3_RX</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -464,7 +478,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -496,9 +510,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -530,6 +545,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -705,14 +721,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
@@ -723,7 +737,7 @@
     <col min="13" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1">
+    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -759,7 +773,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>23</v>
       </c>
@@ -783,7 +797,7 @@
       </c>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>24</v>
       </c>
@@ -800,7 +814,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>69</v>
       </c>
@@ -819,12 +833,12 @@
       <c r="J4" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="K4" s="2">
+      <c r="K4" s="2"/>
+      <c r="L4" s="2">
         <v>41</v>
       </c>
-      <c r="L4" s="2"/>
-    </row>
-    <row r="5" spans="1:12">
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>70</v>
       </c>
@@ -843,10 +857,12 @@
       <c r="J5" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="K5" s="2"/>
+      <c r="K5" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="L5" s="2"/>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>25</v>
       </c>
@@ -864,7 +880,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>31</v>
       </c>
@@ -888,7 +904,7 @@
       </c>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>32</v>
       </c>
@@ -905,7 +921,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>67</v>
       </c>
@@ -922,7 +938,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>68</v>
       </c>
@@ -943,12 +959,12 @@
       <c r="J10" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="K10" s="2">
+      <c r="K10" s="2"/>
+      <c r="L10" s="2">
         <v>44</v>
       </c>
-      <c r="L10" s="2"/>
-    </row>
-    <row r="11" spans="1:12">
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>96</v>
       </c>
@@ -972,7 +988,7 @@
       </c>
       <c r="L11" s="2"/>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>47</v>
       </c>
@@ -994,16 +1010,13 @@
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>48</v>
       </c>
       <c r="B13" t="s">
         <v>13</v>
       </c>
-      <c r="D13" t="s">
-        <v>105</v>
-      </c>
       <c r="E13" t="s">
         <v>53</v>
       </c>
@@ -1014,7 +1027,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>51</v>
       </c>
@@ -1028,7 +1041,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>52</v>
       </c>
@@ -1045,7 +1058,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>90</v>
       </c>
@@ -1062,7 +1075,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>92</v>
       </c>
@@ -1090,7 +1103,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>93</v>
       </c>
@@ -1113,7 +1126,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>95</v>
       </c>
@@ -1133,7 +1146,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>96</v>
       </c>
@@ -1157,7 +1170,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>66</v>
       </c>
@@ -1174,231 +1187,275 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
-      <c r="A22" s="2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>56</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C22" s="4"/>
+      <c r="D22" t="s">
+        <v>106</v>
+      </c>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4">
+        <v>41</v>
+      </c>
+      <c r="L22" s="4"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>58</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C23" s="4"/>
+      <c r="D23" t="s">
+        <v>105</v>
+      </c>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4">
+        <v>43</v>
+      </c>
+      <c r="L23" s="4"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
         <v>59</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B24" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="K22" s="2">
-        <v>44</v>
-      </c>
-      <c r="L22" s="2"/>
-    </row>
-    <row r="23" spans="1:12">
-      <c r="A23" s="2">
-        <v>60</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="K23" s="2">
-        <v>45</v>
-      </c>
-      <c r="L23" s="2"/>
-    </row>
-    <row r="24" spans="1:12">
-      <c r="A24" s="2">
-        <v>61</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>96</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="K24" s="2">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="L24" s="2"/>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="K25" s="2">
+        <v>45</v>
+      </c>
+      <c r="L25" s="2"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>61</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="K26" s="2">
+        <v>46</v>
+      </c>
+      <c r="L26" s="2"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>62</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="K25" s="2">
+      <c r="K27" s="2">
         <v>47</v>
       </c>
-      <c r="L25" s="2"/>
-    </row>
-    <row r="26" spans="1:12">
-      <c r="A26">
+      <c r="L27" s="2"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28">
         <v>42</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B28" t="s">
         <v>32</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D28" t="s">
         <v>108</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E28" t="s">
         <v>33</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F28" t="s">
         <v>33</v>
       </c>
-      <c r="K26">
+      <c r="K28">
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
-      <c r="A27">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29">
         <v>44</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B29" t="s">
         <v>37</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D29" t="s">
         <v>107</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E29" t="s">
         <v>36</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F29" t="s">
         <v>36</v>
       </c>
-      <c r="K27">
+      <c r="K29">
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
-      <c r="A28">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30">
         <v>45</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B30" t="s">
         <v>40</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D30" t="s">
         <v>109</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E30" t="s">
         <v>39</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F30" t="s">
         <v>39</v>
       </c>
-      <c r="K28">
+      <c r="K30">
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
-      <c r="A29">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31">
         <v>46</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B31" t="s">
         <v>67</v>
       </c>
-      <c r="D29" t="s">
-        <v>106</v>
-      </c>
-      <c r="K29">
+      <c r="D31" s="4"/>
+      <c r="K31">
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
-      <c r="A30">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32">
         <v>39</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B32" t="s">
         <v>31</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E32" t="s">
         <v>53</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F32" t="s">
         <v>51</v>
       </c>
-      <c r="K30">
+      <c r="K32">
         <v>39</v>
       </c>
     </row>
-    <row r="31" spans="1:12">
-      <c r="A31">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33">
         <v>40</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B33" t="s">
         <v>52</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E33" t="s">
         <v>28</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F33" t="s">
         <v>28</v>
       </c>
-      <c r="K31">
+      <c r="K33">
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:12">
-      <c r="A32" s="2">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
         <v>30</v>
       </c>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2" t="s">
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
-      <c r="J32" s="2" t="s">
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="K32" s="2">
+      <c r="K34" s="2">
         <v>15</v>
       </c>
-      <c r="L32" s="2"/>
+      <c r="L34" s="2"/>
     </row>
   </sheetData>
   <sortState ref="A2:L35">
@@ -1410,20 +1467,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>44</v>
       </c>
@@ -1431,7 +1488,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>45</v>
       </c>
@@ -1439,7 +1496,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>46</v>
       </c>
@@ -1447,7 +1504,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>65</v>
       </c>
@@ -1455,7 +1512,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>66</v>
       </c>
@@ -1463,7 +1520,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>47</v>
       </c>
@@ -1471,7 +1528,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>89</v>
       </c>
@@ -1486,18 +1543,18 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>71</v>
       </c>
@@ -1526,7 +1583,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>80</v>
       </c>
@@ -1534,22 +1591,22 @@
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>84</v>
       </c>
@@ -1557,17 +1614,17 @@
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>87</v>
       </c>

</xml_diff>

<commit_message>
added no connects to mcu connectors
</commit_message>
<xml_diff>
--- a/docs/crossbar.xlsx
+++ b/docs/crossbar.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="137">
   <si>
     <t>PB10</t>
   </si>
@@ -404,9 +404,6 @@
     <t>PC4</t>
   </si>
   <si>
-    <t>SCL</t>
-  </si>
-  <si>
     <t>CLK</t>
   </si>
   <si>
@@ -432,6 +429,9 @@
   </si>
   <si>
     <t>CS_SDA</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -791,10 +791,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M49"/>
+  <dimension ref="A1:M48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -836,7 +836,7 @@
         <v>48</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>17</v>
@@ -936,9 +936,11 @@
         <v>41</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="M5" s="2"/>
+        <v>136</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -1079,7 +1081,7 @@
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
@@ -1091,674 +1093,649 @@
       <c r="M12" s="4"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <v>92</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2">
-        <v>23</v>
+      <c r="A13">
+        <v>90</v>
+      </c>
+      <c r="B13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13" t="s">
+        <v>62</v>
+      </c>
+      <c r="G13" t="s">
+        <v>62</v>
+      </c>
+      <c r="M13">
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>47</v>
+        <v>92</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
+      <c r="G14" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="H14" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I14" s="2"/>
+        <v>7</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="J14" s="2"/>
       <c r="K14" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="L14" s="2">
-        <v>34</v>
-      </c>
-      <c r="M14" s="2"/>
+        <v>20</v>
+      </c>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2">
+        <v>23</v>
+      </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>48</v>
+        <v>93</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="D15" t="s">
+        <v>135</v>
       </c>
       <c r="E15" t="s">
-        <v>52</v>
+        <v>15</v>
+      </c>
+      <c r="G15" t="s">
+        <v>92</v>
       </c>
       <c r="H15" t="s">
-        <v>16</v>
-      </c>
-      <c r="L15">
-        <v>35</v>
+        <v>15</v>
+      </c>
+      <c r="M15">
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>51</v>
+        <v>95</v>
       </c>
       <c r="B16" t="s">
-        <v>67</v>
+        <v>8</v>
+      </c>
+      <c r="D16" t="s">
+        <v>134</v>
       </c>
       <c r="E16" t="s">
+        <v>7</v>
+      </c>
+      <c r="G16" t="s">
+        <v>94</v>
+      </c>
+      <c r="H16" t="s">
+        <v>7</v>
+      </c>
+      <c r="M16">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>96</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>47</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="L18" s="2">
+        <v>34</v>
+      </c>
+      <c r="M18" s="2"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>48</v>
+      </c>
+      <c r="B19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" t="s">
         <v>52</v>
       </c>
-      <c r="L16">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>52</v>
-      </c>
-      <c r="B17" t="s">
-        <v>28</v>
-      </c>
-      <c r="E17" t="s">
-        <v>52</v>
-      </c>
-      <c r="F17" t="s">
-        <v>50</v>
-      </c>
-      <c r="L17">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>90</v>
-      </c>
-      <c r="B18" t="s">
-        <v>63</v>
-      </c>
-      <c r="E18" t="s">
-        <v>62</v>
-      </c>
-      <c r="G18" t="s">
-        <v>62</v>
-      </c>
-      <c r="M18">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
-        <v>92</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2">
-        <v>23</v>
+      <c r="H19" t="s">
+        <v>16</v>
+      </c>
+      <c r="L19">
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>93</v>
+        <v>51</v>
       </c>
       <c r="B20" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20" t="s">
-        <v>136</v>
+        <v>67</v>
       </c>
       <c r="E20" t="s">
-        <v>15</v>
-      </c>
-      <c r="G20" t="s">
-        <v>92</v>
-      </c>
-      <c r="H20" t="s">
-        <v>15</v>
-      </c>
-      <c r="M20">
-        <v>24</v>
+        <v>52</v>
+      </c>
+      <c r="L20">
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>95</v>
+        <v>52</v>
       </c>
       <c r="B21" t="s">
-        <v>8</v>
-      </c>
-      <c r="D21" t="s">
-        <v>135</v>
+        <v>28</v>
       </c>
       <c r="E21" t="s">
-        <v>7</v>
-      </c>
-      <c r="G21" t="s">
-        <v>94</v>
-      </c>
-      <c r="H21" t="s">
-        <v>7</v>
-      </c>
-      <c r="M21">
-        <v>19</v>
+        <v>52</v>
+      </c>
+      <c r="F21" t="s">
+        <v>50</v>
+      </c>
+      <c r="L21">
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <v>96</v>
+        <v>15</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>98</v>
+        <v>120</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
-      <c r="G22" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="L22" s="2"/>
-      <c r="M22" s="2">
-        <v>20</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="L22" s="2">
+        <v>8</v>
+      </c>
+      <c r="M22" s="2"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
-        <v>15</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="L23" s="2">
-        <v>8</v>
-      </c>
-      <c r="M23" s="2"/>
+      <c r="A23">
+        <v>17</v>
+      </c>
+      <c r="B23" t="s">
+        <v>122</v>
+      </c>
+      <c r="L23">
+        <v>10</v>
+      </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="B24" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="L24">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="B25" t="s">
-        <v>126</v>
-      </c>
-      <c r="L25">
-        <v>20</v>
+        <v>129</v>
+      </c>
+      <c r="G25" t="s">
+        <v>62</v>
+      </c>
+      <c r="H25" t="s">
+        <v>130</v>
+      </c>
+      <c r="K25" t="s">
+        <v>132</v>
+      </c>
+      <c r="M25">
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B26" t="s">
-        <v>130</v>
-      </c>
-      <c r="G26" t="s">
-        <v>62</v>
+        <v>10</v>
+      </c>
+      <c r="E26" t="s">
+        <v>52</v>
       </c>
       <c r="H26" t="s">
-        <v>131</v>
-      </c>
-      <c r="K26" t="s">
-        <v>133</v>
+        <v>14</v>
       </c>
       <c r="M26">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>66</v>
-      </c>
-      <c r="B27" t="s">
-        <v>10</v>
-      </c>
-      <c r="E27" t="s">
-        <v>52</v>
-      </c>
-      <c r="H27" t="s">
-        <v>14</v>
-      </c>
-      <c r="M27">
-        <v>46</v>
+      <c r="A27" s="2">
+        <v>8</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2">
+        <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
-        <v>8</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="L28" s="2"/>
-      <c r="M28" s="2">
-        <v>9</v>
-      </c>
+      <c r="A28" s="4">
+        <v>56</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C28" s="4"/>
+      <c r="D28" t="s">
+        <v>105</v>
+      </c>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4">
+        <v>41</v>
+      </c>
+      <c r="M28" s="4"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C29" s="4"/>
       <c r="D29" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
-      <c r="I29" s="4" t="s">
-        <v>112</v>
-      </c>
+      <c r="I29" s="4"/>
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
       <c r="L29" s="4">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="M29" s="4"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="4">
-        <v>58</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="C30" s="4"/>
-      <c r="D30" t="s">
-        <v>104</v>
-      </c>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="4"/>
-      <c r="J30" s="4"/>
-      <c r="K30" s="4"/>
-      <c r="L30" s="4">
-        <v>43</v>
-      </c>
-      <c r="M30" s="4"/>
+      <c r="A30" s="2">
+        <v>59</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="L30" s="2">
+        <v>44</v>
+      </c>
+      <c r="M30" s="2"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
       <c r="K31" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="L31" s="2">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="M31" s="2"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
       <c r="K32" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="L32" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M32" s="2"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
       <c r="G33" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
       <c r="K33" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="L33" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="M33" s="2"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
-        <v>62</v>
+        <v>97</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>97</v>
+        <v>118</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
-      <c r="G34" s="2" t="s">
-        <v>96</v>
-      </c>
+      <c r="G34" s="2"/>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
       <c r="K34" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="L34" s="2">
-        <v>47</v>
-      </c>
-      <c r="M34" s="2"/>
+        <v>119</v>
+      </c>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2">
+        <v>17</v>
+      </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" s="2">
-        <v>97</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
-      <c r="J35" s="2"/>
-      <c r="K35" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="L35" s="2"/>
-      <c r="M35" s="2">
-        <v>17</v>
+      <c r="A35">
+        <v>1</v>
+      </c>
+      <c r="B35" t="s">
+        <v>117</v>
+      </c>
+      <c r="D35" t="s">
+        <v>133</v>
+      </c>
+      <c r="E35" t="s">
+        <v>52</v>
+      </c>
+      <c r="M35">
+        <v>15</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B36" t="s">
-        <v>117</v>
-      </c>
-      <c r="D36" t="s">
-        <v>134</v>
-      </c>
-      <c r="E36" t="s">
-        <v>52</v>
+        <v>116</v>
       </c>
       <c r="M36">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B37" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M37">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>5</v>
+        <v>42</v>
       </c>
       <c r="B38" t="s">
-        <v>115</v>
-      </c>
-      <c r="M38">
-        <v>11</v>
+        <v>31</v>
+      </c>
+      <c r="D38" t="s">
+        <v>107</v>
+      </c>
+      <c r="E38" t="s">
+        <v>32</v>
+      </c>
+      <c r="F38" t="s">
+        <v>32</v>
+      </c>
+      <c r="L38">
+        <v>29</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B39" t="s">
+        <v>36</v>
+      </c>
+      <c r="D39" t="s">
+        <v>106</v>
+      </c>
+      <c r="E39" t="s">
+        <v>35</v>
+      </c>
+      <c r="F39" t="s">
+        <v>35</v>
+      </c>
+      <c r="L39">
         <v>31</v>
-      </c>
-      <c r="D39" t="s">
-        <v>107</v>
-      </c>
-      <c r="E39" t="s">
-        <v>32</v>
-      </c>
-      <c r="F39" t="s">
-        <v>32</v>
-      </c>
-      <c r="L39">
-        <v>29</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B40" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D40" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E40" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F40" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="L40">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B41" t="s">
-        <v>39</v>
-      </c>
-      <c r="D41" t="s">
-        <v>108</v>
-      </c>
-      <c r="E41" t="s">
-        <v>38</v>
-      </c>
-      <c r="F41" t="s">
-        <v>38</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="D41" s="4"/>
       <c r="L41">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B42" t="s">
-        <v>66</v>
-      </c>
-      <c r="D42" s="4"/>
+        <v>30</v>
+      </c>
+      <c r="E42" t="s">
+        <v>52</v>
+      </c>
+      <c r="F42" t="s">
+        <v>50</v>
+      </c>
       <c r="L42">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B43" t="s">
+        <v>51</v>
+      </c>
+      <c r="E43" t="s">
+        <v>27</v>
+      </c>
+      <c r="F43" t="s">
+        <v>27</v>
+      </c>
+      <c r="L43">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
         <v>30</v>
       </c>
-      <c r="E43" t="s">
-        <v>52</v>
-      </c>
-      <c r="F43" t="s">
-        <v>50</v>
-      </c>
-      <c r="L43">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>40</v>
-      </c>
-      <c r="B44" t="s">
-        <v>51</v>
-      </c>
-      <c r="E44" t="s">
-        <v>27</v>
-      </c>
-      <c r="F44" t="s">
-        <v>27</v>
-      </c>
-      <c r="L44">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A45" s="2">
-        <v>30</v>
-      </c>
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2"/>
-      <c r="F45" s="2" t="s">
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="G45" s="2"/>
-      <c r="H45" s="2"/>
-      <c r="I45" s="2"/>
-      <c r="J45" s="2"/>
-      <c r="K45" s="2" t="s">
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="L45" s="2">
+      <c r="L44" s="2">
         <v>15</v>
       </c>
-      <c r="M45" s="2"/>
-    </row>
-    <row r="49" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D49" t="s">
+      <c r="M44" s="2"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D48" t="s">
         <v>109</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E48" t="s">
         <v>15</v>
       </c>
-      <c r="G49" t="s">
+      <c r="G48" t="s">
         <v>92</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added LED USART to layout
</commit_message>
<xml_diff>
--- a/docs/crossbar.xlsx
+++ b/docs/crossbar.xlsx
@@ -16,12 +16,12 @@
     <sheet name="Peripherals" sheetId="2" r:id="rId2"/>
     <sheet name="DMA" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="144">
   <si>
     <t>PB10</t>
   </si>
@@ -432,6 +432,27 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>PD5</t>
+  </si>
+  <si>
+    <t>OverCurrent</t>
+  </si>
+  <si>
+    <t>TIM2_CH3</t>
+  </si>
+  <si>
+    <t>TIM5_CH3</t>
+  </si>
+  <si>
+    <t>AF3</t>
+  </si>
+  <si>
+    <t>TIM9_CH1</t>
+  </si>
+  <si>
+    <t>LED_USART</t>
   </si>
 </sst>
 </file>
@@ -791,10 +812,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M48"/>
+  <dimension ref="A1:N49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -803,13 +824,14 @@
     <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" customWidth="1"/>
-    <col min="11" max="11" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="4"/>
+    <col min="8" max="8" width="10" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -830,25 +852,28 @@
         <v>25</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>23</v>
       </c>
@@ -865,15 +890,16 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="2"/>
+      <c r="L2" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="L2" s="2">
+      <c r="M2" s="2">
         <v>12</v>
       </c>
-      <c r="M2" s="2"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N2" s="2"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>24</v>
       </c>
@@ -886,11 +912,11 @@
       <c r="F3" t="s">
         <v>58</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>69</v>
       </c>
@@ -907,15 +933,16 @@
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
-      <c r="K4" s="2" t="s">
+      <c r="K4" s="2"/>
+      <c r="L4" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2">
+      <c r="M4" s="2"/>
+      <c r="N4" s="2">
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>70</v>
       </c>
@@ -932,35 +959,47 @@
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
-      <c r="K5" s="2" t="s">
+      <c r="K5" s="2"/>
+      <c r="L5" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>136</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N5" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>25</v>
       </c>
       <c r="B6" t="s">
         <v>68</v>
       </c>
-      <c r="D6" s="4"/>
+      <c r="D6" s="4" t="s">
+        <v>143</v>
+      </c>
       <c r="E6" t="s">
         <v>69</v>
       </c>
-      <c r="I6" t="s">
+      <c r="F6" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="G6" t="s">
+        <v>140</v>
+      </c>
+      <c r="H6" t="s">
+        <v>142</v>
+      </c>
+      <c r="J6" t="s">
         <v>69</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>29</v>
       </c>
@@ -975,15 +1014,16 @@
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="2" t="s">
+      <c r="K7" s="2"/>
+      <c r="L7" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="L7" s="2">
+      <c r="M7" s="2">
         <v>16</v>
       </c>
-      <c r="M7" s="2"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N7" s="2"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>31</v>
       </c>
@@ -1000,15 +1040,16 @@
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
-      <c r="K8" s="2" t="s">
+      <c r="K8" s="2"/>
+      <c r="L8" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="L8" s="2">
+      <c r="M8" s="2">
         <v>18</v>
       </c>
-      <c r="M8" s="2"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N8" s="2"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>32</v>
       </c>
@@ -1018,14 +1059,14 @@
       <c r="G9" t="s">
         <v>26</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>40</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>67</v>
       </c>
@@ -1035,14 +1076,14 @@
       <c r="F10" t="s">
         <v>27</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>3</v>
       </c>
-      <c r="M10">
+      <c r="N10">
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>68</v>
       </c>
@@ -1057,19 +1098,20 @@
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
-      <c r="I11" s="2" t="s">
+      <c r="I11" s="2"/>
+      <c r="J11" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2" t="s">
+      <c r="K11" s="2"/>
+      <c r="L11" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2">
+      <c r="M11" s="2"/>
+      <c r="N11" s="2">
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>36</v>
       </c>
@@ -1087,12 +1129,13 @@
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
-      <c r="L12" s="4">
+      <c r="L12" s="4"/>
+      <c r="M12" s="4">
         <v>22</v>
       </c>
-      <c r="M12" s="4"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N12" s="4"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>90</v>
       </c>
@@ -1105,11 +1148,11 @@
       <c r="G13" t="s">
         <v>62</v>
       </c>
-      <c r="M13">
+      <c r="N13">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>92</v>
       </c>
@@ -1123,22 +1166,23 @@
       <c r="G14" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="H14" s="2"/>
+      <c r="I14" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="J14" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2" t="s">
+      <c r="K14" s="2"/>
+      <c r="L14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2">
+      <c r="M14" s="2"/>
+      <c r="N14" s="2">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>93</v>
       </c>
@@ -1154,14 +1198,14 @@
       <c r="G15" t="s">
         <v>92</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
         <v>15</v>
       </c>
-      <c r="M15">
+      <c r="N15">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>95</v>
       </c>
@@ -1177,14 +1221,14 @@
       <c r="G16" t="s">
         <v>94</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I16" t="s">
         <v>7</v>
       </c>
-      <c r="M16">
+      <c r="N16">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>96</v>
       </c>
@@ -1198,20 +1242,21 @@
       <c r="G17" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="H17" s="2" t="s">
+      <c r="H17" s="2"/>
+      <c r="I17" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I17" s="2"/>
       <c r="J17" s="2"/>
-      <c r="K17" s="2" t="s">
+      <c r="K17" s="2"/>
+      <c r="L17" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2">
+      <c r="M17" s="2"/>
+      <c r="N17" s="2">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>47</v>
       </c>
@@ -1223,20 +1268,21 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
-      <c r="H18" s="2" t="s">
+      <c r="H18" s="2"/>
+      <c r="I18" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I18" s="2"/>
       <c r="J18" s="2"/>
-      <c r="K18" s="2" t="s">
+      <c r="K18" s="2"/>
+      <c r="L18" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="L18" s="2">
+      <c r="M18" s="2">
         <v>34</v>
       </c>
-      <c r="M18" s="2"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N18" s="2"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>48</v>
       </c>
@@ -1246,14 +1292,14 @@
       <c r="E19" t="s">
         <v>52</v>
       </c>
-      <c r="H19" t="s">
+      <c r="I19" t="s">
         <v>16</v>
       </c>
-      <c r="L19">
+      <c r="M19">
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>51</v>
       </c>
@@ -1263,11 +1309,11 @@
       <c r="E20" t="s">
         <v>52</v>
       </c>
-      <c r="L20">
+      <c r="M20">
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>52</v>
       </c>
@@ -1280,11 +1326,11 @@
       <c r="F21" t="s">
         <v>50</v>
       </c>
-      <c r="L21">
+      <c r="M21">
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>15</v>
       </c>
@@ -1299,37 +1345,38 @@
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
-      <c r="K22" s="2" t="s">
+      <c r="K22" s="2"/>
+      <c r="L22" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="L22" s="2">
+      <c r="M22" s="2">
         <v>8</v>
       </c>
-      <c r="M22" s="2"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N22" s="2"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>17</v>
       </c>
       <c r="B23" t="s">
         <v>122</v>
       </c>
-      <c r="L23">
+      <c r="M23">
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>33</v>
       </c>
       <c r="B24" t="s">
         <v>126</v>
       </c>
-      <c r="L24">
+      <c r="M24">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>63</v>
       </c>
@@ -1339,17 +1386,17 @@
       <c r="G25" t="s">
         <v>62</v>
       </c>
-      <c r="H25" t="s">
+      <c r="I25" t="s">
         <v>130</v>
       </c>
-      <c r="K25" t="s">
+      <c r="L25" t="s">
         <v>132</v>
       </c>
-      <c r="M25">
+      <c r="N25">
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>66</v>
       </c>
@@ -1359,14 +1406,14 @@
       <c r="E26" t="s">
         <v>52</v>
       </c>
-      <c r="H26" t="s">
+      <c r="I26" t="s">
         <v>14</v>
       </c>
-      <c r="M26">
+      <c r="N26">
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>8</v>
       </c>
@@ -1381,361 +1428,396 @@
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
-      <c r="K27" s="2" t="s">
+      <c r="K27" s="2"/>
+      <c r="L27" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="L27" s="2"/>
-      <c r="M27" s="2">
+      <c r="M27" s="2"/>
+      <c r="N27" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="4">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>86</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
         <v>56</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B29" s="4" t="s">
         <v>111</v>
-      </c>
-      <c r="C28" s="4"/>
-      <c r="D28" t="s">
-        <v>105</v>
-      </c>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
-      <c r="L28" s="4">
-        <v>41</v>
-      </c>
-      <c r="M28" s="4"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="4">
-        <v>58</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>110</v>
       </c>
       <c r="C29" s="4"/>
       <c r="D29" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
-      <c r="J29" s="4"/>
+      <c r="J29" s="4" t="s">
+        <v>112</v>
+      </c>
       <c r="K29" s="4"/>
-      <c r="L29" s="4">
+      <c r="L29" s="4"/>
+      <c r="M29" s="4">
+        <v>41</v>
+      </c>
+      <c r="N29" s="4"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
+        <v>58</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C30" s="4"/>
+      <c r="D30" t="s">
+        <v>104</v>
+      </c>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
+      <c r="M30" s="4">
         <v>43</v>
       </c>
-      <c r="M29" s="4"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
+      <c r="N30" s="4"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
         <v>59</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B31" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="L30" s="2">
-        <v>44</v>
-      </c>
-      <c r="M30" s="2"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
-        <v>60</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>93</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
-      <c r="K31" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="L31" s="2">
-        <v>45</v>
-      </c>
-      <c r="M31" s="2"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K31" s="2"/>
+      <c r="L31" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="M31" s="2">
+        <v>44</v>
+      </c>
+      <c r="N31" s="2"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
-      <c r="K32" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="L32" s="2">
-        <v>46</v>
-      </c>
-      <c r="M32" s="2"/>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K32" s="2"/>
+      <c r="L32" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="M32" s="2">
+        <v>45</v>
+      </c>
+      <c r="N32" s="2"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
       <c r="G33" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
-      <c r="K33" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="L33" s="2">
-        <v>47</v>
-      </c>
-      <c r="M33" s="2"/>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K33" s="2"/>
+      <c r="L33" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="M33" s="2">
+        <v>46</v>
+      </c>
+      <c r="N33" s="2"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
+        <v>62</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>118</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
+      <c r="G34" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
-      <c r="K34" s="2" t="s">
+      <c r="K34" s="2"/>
+      <c r="L34" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="M34" s="2">
+        <v>47</v>
+      </c>
+      <c r="N34" s="2"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>97</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="L34" s="2"/>
-      <c r="M34" s="2">
+      <c r="M35" s="2"/>
+      <c r="N35" s="2">
         <v>17</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36">
         <v>1</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>117</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D36" t="s">
         <v>133</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E36" t="s">
         <v>52</v>
       </c>
-      <c r="M35">
+      <c r="N36">
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A37">
         <v>3</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>116</v>
       </c>
-      <c r="M36">
+      <c r="N37">
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A38">
         <v>5</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>115</v>
       </c>
-      <c r="M37">
+      <c r="N38">
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A38">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A39">
         <v>42</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>31</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D39" t="s">
         <v>107</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E39" t="s">
         <v>32</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F39" t="s">
         <v>32</v>
       </c>
-      <c r="L38">
+      <c r="M39">
         <v>29</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A40">
         <v>44</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B40" t="s">
         <v>36</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D40" t="s">
         <v>106</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E40" t="s">
         <v>35</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F40" t="s">
         <v>35</v>
       </c>
-      <c r="L39">
+      <c r="M40">
         <v>31</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A40">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A41">
         <v>45</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B41" t="s">
         <v>39</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D41" t="s">
         <v>108</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E41" t="s">
         <v>38</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F41" t="s">
         <v>38</v>
       </c>
-      <c r="L40">
+      <c r="M41">
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A41">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A42">
         <v>46</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B42" t="s">
         <v>66</v>
       </c>
-      <c r="D41" s="4"/>
-      <c r="L41">
+      <c r="D42" s="4"/>
+      <c r="M42">
         <v>33</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A42">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A43">
         <v>39</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B43" t="s">
         <v>30</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E43" t="s">
         <v>52</v>
       </c>
-      <c r="F42" t="s">
+      <c r="F43" t="s">
         <v>50</v>
       </c>
-      <c r="L42">
+      <c r="M43">
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A43">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A44">
         <v>40</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B44" t="s">
         <v>51</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E44" t="s">
         <v>27</v>
       </c>
-      <c r="F43" t="s">
+      <c r="F44" t="s">
         <v>27</v>
       </c>
-      <c r="L43">
+      <c r="M44">
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A44" s="2">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A45" s="2">
         <v>30</v>
       </c>
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
-      <c r="E44" s="2"/>
-      <c r="F44" s="2" t="s">
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="G44" s="2"/>
-      <c r="H44" s="2"/>
-      <c r="I44" s="2"/>
-      <c r="J44" s="2"/>
-      <c r="K44" s="2" t="s">
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
+      <c r="L45" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="L44" s="2">
+      <c r="M45" s="2">
         <v>15</v>
       </c>
-      <c r="M44" s="2"/>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D48" t="s">
+      <c r="N45" s="2"/>
+    </row>
+    <row r="49" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D49" t="s">
         <v>109</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E49" t="s">
         <v>15</v>
       </c>
-      <c r="G48" t="s">
+      <c r="G49" t="s">
         <v>92</v>
       </c>
     </row>
@@ -1753,7 +1835,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added fan driver components to layout
</commit_message>
<xml_diff>
--- a/docs/crossbar.xlsx
+++ b/docs/crossbar.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="145">
   <si>
     <t>PB10</t>
   </si>
@@ -453,6 +453,9 @@
   </si>
   <si>
     <t>LED_USART</t>
+  </si>
+  <si>
+    <t>FAN</t>
   </si>
 </sst>
 </file>
@@ -815,7 +818,7 @@
   <dimension ref="A1:N49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -906,6 +909,9 @@
       <c r="B3" t="s">
         <v>57</v>
       </c>
+      <c r="D3" t="s">
+        <v>144</v>
+      </c>
       <c r="E3" t="s">
         <v>58</v>
       </c>
@@ -1834,8 +1840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added pump parts to layout
</commit_message>
<xml_diff>
--- a/docs/crossbar.xlsx
+++ b/docs/crossbar.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="148">
   <si>
     <t>PB10</t>
   </si>
@@ -456,6 +456,15 @@
   </si>
   <si>
     <t>FAN</t>
+  </si>
+  <si>
+    <t>PB0</t>
+  </si>
+  <si>
+    <t>TIM3_CH3</t>
+  </si>
+  <si>
+    <t>PUMP</t>
   </si>
 </sst>
 </file>
@@ -815,11 +824,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N49"/>
+  <dimension ref="A1:N50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1119,17 +1126,17 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>12</v>
+        <v>145</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4" t="s">
-        <v>128</v>
+        <v>146</v>
       </c>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
@@ -1142,313 +1149,314 @@
       <c r="N12" s="4"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="A13" s="4">
+        <v>36</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4">
+        <v>21</v>
+      </c>
+      <c r="N13" s="4"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>90</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>63</v>
       </c>
-      <c r="E13" t="s">
+      <c r="G14" t="s">
         <v>62</v>
       </c>
-      <c r="G13" t="s">
-        <v>62</v>
-      </c>
-      <c r="N13">
+      <c r="N14">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
         <v>92</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B15" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2" t="s">
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2" t="s">
+      <c r="H15" s="2"/>
+      <c r="I15" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J14" s="2" t="s">
+      <c r="J15" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2" t="s">
+      <c r="K15" s="2"/>
+      <c r="L15" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2">
+      <c r="M15" s="2"/>
+      <c r="N15" s="2">
         <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>93</v>
-      </c>
-      <c r="B15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" t="s">
-        <v>135</v>
-      </c>
-      <c r="E15" t="s">
-        <v>15</v>
-      </c>
-      <c r="G15" t="s">
-        <v>92</v>
-      </c>
-      <c r="I15" t="s">
-        <v>15</v>
-      </c>
-      <c r="N15">
-        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
+        <v>93</v>
+      </c>
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" t="s">
+        <v>135</v>
+      </c>
+      <c r="E16" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" t="s">
+        <v>92</v>
+      </c>
+      <c r="I16" t="s">
+        <v>15</v>
+      </c>
+      <c r="N16">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17">
         <v>95</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>8</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D17" t="s">
         <v>134</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E17" t="s">
         <v>7</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G17" t="s">
         <v>94</v>
       </c>
-      <c r="I16" t="s">
+      <c r="I17" t="s">
         <v>7</v>
       </c>
-      <c r="N16">
+      <c r="N17">
         <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
-        <v>96</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2">
-        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>47</v>
+        <v>96</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
+      <c r="G18" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="H18" s="2"/>
       <c r="I18" s="2" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
       <c r="L18" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>47</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="M18" s="2">
+      <c r="M19" s="2">
         <v>34</v>
       </c>
-      <c r="N18" s="2"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>48</v>
-      </c>
-      <c r="B19" t="s">
-        <v>13</v>
-      </c>
-      <c r="E19" t="s">
-        <v>52</v>
-      </c>
-      <c r="I19" t="s">
-        <v>16</v>
-      </c>
-      <c r="M19">
-        <v>35</v>
-      </c>
+      <c r="N19" s="2"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B20" t="s">
-        <v>67</v>
+        <v>13</v>
       </c>
       <c r="E20" t="s">
         <v>52</v>
       </c>
+      <c r="I20" t="s">
+        <v>16</v>
+      </c>
       <c r="M20">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B21" t="s">
-        <v>28</v>
+        <v>67</v>
       </c>
       <c r="E21" t="s">
         <v>52</v>
       </c>
-      <c r="F21" t="s">
+      <c r="M21">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>52</v>
+      </c>
+      <c r="B22" t="s">
+        <v>28</v>
+      </c>
+      <c r="E22" t="s">
+        <v>52</v>
+      </c>
+      <c r="F22" t="s">
         <v>50</v>
       </c>
-      <c r="M21">
+      <c r="M22">
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
         <v>15</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B23" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="2" t="s">
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="M22" s="2">
+      <c r="M23" s="2">
         <v>8</v>
       </c>
-      <c r="N22" s="2"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>17</v>
-      </c>
-      <c r="B23" t="s">
-        <v>122</v>
-      </c>
-      <c r="M23">
-        <v>10</v>
-      </c>
+      <c r="N23" s="2"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="B24" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="M24">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>63</v>
+        <v>33</v>
       </c>
       <c r="B25" t="s">
-        <v>129</v>
-      </c>
-      <c r="G25" t="s">
-        <v>62</v>
-      </c>
-      <c r="I25" t="s">
-        <v>130</v>
-      </c>
-      <c r="L25" t="s">
-        <v>132</v>
-      </c>
-      <c r="N25">
-        <v>47</v>
+        <v>126</v>
+      </c>
+      <c r="M25">
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26">
+        <v>63</v>
+      </c>
+      <c r="B26" t="s">
+        <v>129</v>
+      </c>
+      <c r="G26" t="s">
+        <v>62</v>
+      </c>
+      <c r="I26" t="s">
+        <v>130</v>
+      </c>
+      <c r="L26" t="s">
+        <v>132</v>
+      </c>
+      <c r="N26">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27">
         <v>66</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>10</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E27" t="s">
         <v>52</v>
       </c>
-      <c r="I26" t="s">
+      <c r="I27" t="s">
         <v>14</v>
       </c>
-      <c r="N26">
+      <c r="N27">
         <v>46</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
-        <v>8</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
-      <c r="L27" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="M27" s="2"/>
-      <c r="N27" s="2">
-        <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
-        <v>86</v>
+        <v>8</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>137</v>
+        <v>113</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -1457,373 +1465,397 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
-      <c r="J28" s="2" t="s">
-        <v>69</v>
-      </c>
+      <c r="J28" s="2"/>
       <c r="K28" s="2"/>
       <c r="L28" s="2" t="s">
-        <v>138</v>
+        <v>114</v>
       </c>
       <c r="M28" s="2"/>
       <c r="N28" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>86</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2">
         <v>29</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="4">
-        <v>56</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="C29" s="4"/>
-      <c r="D29" t="s">
-        <v>105</v>
-      </c>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
-      <c r="I29" s="4"/>
-      <c r="J29" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="K29" s="4"/>
-      <c r="L29" s="4"/>
-      <c r="M29" s="4">
-        <v>41</v>
-      </c>
-      <c r="N29" s="4"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C30" s="4"/>
       <c r="D30" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
-      <c r="J30" s="4"/>
+      <c r="J30" s="4" t="s">
+        <v>112</v>
+      </c>
       <c r="K30" s="4"/>
       <c r="L30" s="4"/>
       <c r="M30" s="4">
+        <v>41</v>
+      </c>
+      <c r="N30" s="4"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
+        <v>58</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C31" s="4"/>
+      <c r="D31" t="s">
+        <v>104</v>
+      </c>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="4"/>
+      <c r="K31" s="4"/>
+      <c r="L31" s="4"/>
+      <c r="M31" s="4">
         <v>43</v>
       </c>
-      <c r="N30" s="4"/>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
-        <v>59</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
-      <c r="L31" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="M31" s="2">
-        <v>44</v>
-      </c>
-      <c r="N31" s="2"/>
+      <c r="N31" s="4"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
       <c r="L32" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="M32" s="2">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N32" s="2"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
       <c r="G33" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
       <c r="L33" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M33" s="2">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="N33" s="2"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
       <c r="G34" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
       <c r="L34" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M34" s="2">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N34" s="2"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
+        <v>62</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>118</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
+      <c r="G35" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
       <c r="L35" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="M35" s="2">
+        <v>47</v>
+      </c>
+      <c r="N35" s="2"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>97</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="M35" s="2"/>
-      <c r="N35" s="2">
+      <c r="M36" s="2"/>
+      <c r="N36" s="2">
         <v>17</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>1</v>
-      </c>
-      <c r="B36" t="s">
-        <v>117</v>
-      </c>
-      <c r="D36" t="s">
-        <v>133</v>
-      </c>
-      <c r="E36" t="s">
-        <v>52</v>
-      </c>
-      <c r="N36">
-        <v>15</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B37" t="s">
-        <v>116</v>
+        <v>117</v>
+      </c>
+      <c r="D37" t="s">
+        <v>133</v>
+      </c>
+      <c r="E37" t="s">
+        <v>52</v>
       </c>
       <c r="N37">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B38" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="N38">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>42</v>
+        <v>5</v>
       </c>
       <c r="B39" t="s">
-        <v>31</v>
-      </c>
-      <c r="D39" t="s">
-        <v>107</v>
-      </c>
-      <c r="E39" t="s">
-        <v>32</v>
-      </c>
-      <c r="F39" t="s">
-        <v>32</v>
-      </c>
-      <c r="M39">
-        <v>29</v>
+        <v>115</v>
+      </c>
+      <c r="N39">
+        <v>11</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B40" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D40" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E40" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F40" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="M40">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B41" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D41" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E41" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F41" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="M41">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B42" t="s">
-        <v>66</v>
-      </c>
-      <c r="D42" s="4"/>
+        <v>39</v>
+      </c>
+      <c r="D42" t="s">
+        <v>108</v>
+      </c>
+      <c r="E42" t="s">
+        <v>38</v>
+      </c>
+      <c r="F42" t="s">
+        <v>38</v>
+      </c>
       <c r="M42">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="B43" t="s">
-        <v>30</v>
-      </c>
-      <c r="E43" t="s">
-        <v>52</v>
-      </c>
-      <c r="F43" t="s">
-        <v>50</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="D43" s="4"/>
       <c r="M43">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44">
+        <v>39</v>
+      </c>
+      <c r="B44" t="s">
+        <v>30</v>
+      </c>
+      <c r="E44" t="s">
+        <v>52</v>
+      </c>
+      <c r="F44" t="s">
+        <v>50</v>
+      </c>
+      <c r="M44">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A45">
         <v>40</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" t="s">
         <v>51</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E45" t="s">
         <v>27</v>
       </c>
-      <c r="F44" t="s">
+      <c r="F45" t="s">
         <v>27</v>
       </c>
-      <c r="M44">
+      <c r="M45">
         <v>27</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A45" s="2">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
         <v>30</v>
       </c>
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2"/>
-      <c r="F45" s="2" t="s">
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="G45" s="2"/>
-      <c r="H45" s="2"/>
-      <c r="I45" s="2"/>
-      <c r="J45" s="2"/>
-      <c r="K45" s="2"/>
-      <c r="L45" s="2" t="s">
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
+      <c r="K46" s="2"/>
+      <c r="L46" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="M45" s="2">
+      <c r="M46" s="2">
         <v>15</v>
       </c>
-      <c r="N45" s="2"/>
-    </row>
-    <row r="49" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D49" t="s">
+      <c r="N46" s="2"/>
+    </row>
+    <row r="50" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D50" t="s">
         <v>109</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E50" t="s">
         <v>15</v>
       </c>
-      <c r="G49" t="s">
+      <c r="G50" t="s">
         <v>92</v>
       </c>
     </row>
@@ -1841,7 +1873,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added hall sensors to layout
</commit_message>
<xml_diff>
--- a/docs/crossbar.xlsx
+++ b/docs/crossbar.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="150">
   <si>
     <t>PB10</t>
   </si>
@@ -465,6 +465,12 @@
   </si>
   <si>
     <t>PUMP</t>
+  </si>
+  <si>
+    <t>HAL_1</t>
+  </si>
+  <si>
+    <t>HAL_2</t>
   </si>
 </sst>
 </file>
@@ -1358,6 +1364,9 @@
       <c r="B22" t="s">
         <v>28</v>
       </c>
+      <c r="D22" t="s">
+        <v>148</v>
+      </c>
       <c r="E22" t="s">
         <v>52</v>
       </c>
@@ -1796,6 +1805,9 @@
       </c>
       <c r="B44" t="s">
         <v>30</v>
+      </c>
+      <c r="D44" t="s">
+        <v>149</v>
       </c>
       <c r="E44" t="s">
         <v>52</v>

</xml_diff>